<commit_message>
mostrar atrasos correctamente y correccion al exportar
</commit_message>
<xml_diff>
--- a/sistema de registro de docentes/Resources/lista_doc.xlsx
+++ b/sistema de registro de docentes/Resources/lista_doc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PROYECTO\proyecto registro de asistencia profesores\sistema de registro de docentes\sistema de registro de docentes\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feros\Source\Repos\sistema_de_registro_de_docentes\sistema de registro de docentes\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F91A71DB-32B0-4524-86CB-D560A4A4CB9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89231EE1-9AED-4C3C-9FC5-520413ABFCAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5115" yWindow="3075" windowWidth="15375" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="5" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="80">
   <si>
     <t>A</t>
   </si>
@@ -104,9 +104,6 @@
     <t xml:space="preserve">FERNANDO </t>
   </si>
   <si>
-    <t xml:space="preserve">579580 Or. </t>
-  </si>
-  <si>
     <t>ANÁLISIS DE CIRCUITOS</t>
   </si>
   <si>
@@ -255,6 +252,27 @@
   </si>
   <si>
     <t>ING. DE SISTEMAS</t>
+  </si>
+  <si>
+    <t>10:00-11:45</t>
+  </si>
+  <si>
+    <t>Viernes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">179580 Or. </t>
+  </si>
+  <si>
+    <t>ingeniero</t>
+  </si>
+  <si>
+    <t>quien</t>
+  </si>
+  <si>
+    <t>soy</t>
+  </si>
+  <si>
+    <t>nose</t>
   </si>
 </sst>
 </file>
@@ -375,7 +393,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
@@ -395,6 +413,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -678,27 +697,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{534D26E8-8FF6-4A1F-B862-3E7EEC9CA17A}">
-  <dimension ref="A1:P19"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.109375" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" customWidth="1"/>
-    <col min="4" max="4" width="17.88671875" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" customWidth="1"/>
-    <col min="6" max="6" width="17.44140625" customWidth="1"/>
-    <col min="7" max="7" width="37.5546875" customWidth="1"/>
-    <col min="8" max="8" width="23.5546875" customWidth="1"/>
-    <col min="9" max="9" width="24.6640625" customWidth="1"/>
-    <col min="16" max="16" width="14.44140625" customWidth="1"/>
-    <col min="17" max="17" width="20.5546875" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="37.5703125" customWidth="1"/>
+    <col min="8" max="8" width="23.5703125" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" customWidth="1"/>
+    <col min="17" max="17" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -721,7 +740,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>6</v>
@@ -739,36 +758,36 @@
         <v>13</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O1" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>0</v>
@@ -780,19 +799,13 @@
         <v>14</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="O2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="M2" s="2"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -809,10 +822,10 @@
         <v>22</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>19</v>
@@ -824,45 +837,43 @@
         <v>4</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="O3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="F4" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="G4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>0</v>
@@ -872,40 +883,40 @@
         <v>15</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>38</v>
       </c>
       <c r="O4" s="1"/>
       <c r="P4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>19</v>
@@ -920,19 +931,17 @@
         <v>15</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="O5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="1:16" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -940,22 +949,22 @@
         <v>18</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
@@ -967,42 +976,40 @@
         <v>14</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="O6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="F7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>0</v>
@@ -1014,30 +1021,30 @@
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>0</v>
@@ -1049,30 +1056,30 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>0</v>
@@ -1084,30 +1091,30 @@
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="H10" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>0</v>
@@ -1119,30 +1126,30 @@
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="G11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>0</v>
@@ -1154,17 +1161,104 @@
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="I12" s="10"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="I14" s="5"/>
-    </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E19" s="5"/>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12">
+        <v>12514210</v>
+      </c>
+      <c r="G12" t="s">
+        <v>65</v>
+      </c>
+      <c r="H12" t="s">
+        <v>59</v>
+      </c>
+      <c r="I12" t="s">
+        <v>0</v>
+      </c>
+      <c r="P12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" t="s">
+        <v>79</v>
+      </c>
+      <c r="F13">
+        <v>12514210</v>
+      </c>
+      <c r="G13" t="s">
+        <v>65</v>
+      </c>
+      <c r="H13" t="s">
+        <v>59</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="P13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F14">
+        <v>12514210</v>
+      </c>
+      <c r="G14" t="s">
+        <v>65</v>
+      </c>
+      <c r="H14" t="s">
+        <v>59</v>
+      </c>
+      <c r="I14" t="s">
+        <v>0</v>
+      </c>
+      <c r="P14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
horarios con filtrado de carrera
</commit_message>
<xml_diff>
--- a/sistema de registro de docentes/Resources/lista_doc.xlsx
+++ b/sistema de registro de docentes/Resources/lista_doc.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Hoja2" sheetId="5" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="190">
   <si>
     <t>Nº</t>
   </si>
@@ -111,6 +111,9 @@
     <t>12:45-14:15</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>CHOQUE</t>
   </si>
   <si>
@@ -171,6 +174,9 @@
     <t>7:45-9:15</t>
   </si>
   <si>
+    <t>Viernes</t>
+  </si>
+  <si>
     <t>MSC</t>
   </si>
   <si>
@@ -231,60 +237,57 @@
     <t>CAMPOS ELECTROMAGNÉTICOS</t>
   </si>
   <si>
-    <t>Viernes</t>
+    <t>PANOZO</t>
+  </si>
+  <si>
+    <t>GONZALES</t>
+  </si>
+  <si>
+    <t>ABIGAIL NOELIA</t>
+  </si>
+  <si>
+    <t>SÍNTESIS DE CIRCUITOS</t>
+  </si>
+  <si>
+    <t>LIC.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VILLA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CABERO </t>
+  </si>
+  <si>
+    <t>MARITZA</t>
+  </si>
+  <si>
+    <t>INVESTIGACIÓN OPERATIVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YAÑIQUEZ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAGNE </t>
+  </si>
+  <si>
+    <t>CLAUDIA</t>
+  </si>
+  <si>
+    <t>PROGRAMACIÓN DE SISTEMAS I</t>
+  </si>
+  <si>
+    <t>12:00-13:30</t>
+  </si>
+  <si>
+    <t>MÉTODOS NUMÉRICOS</t>
+  </si>
+  <si>
+    <t>12:00-14:15</t>
   </si>
   <si>
     <t>11:00-13:30</t>
   </si>
   <si>
-    <t>PANOZO</t>
-  </si>
-  <si>
-    <t>GONZALES</t>
-  </si>
-  <si>
-    <t>ABIGAIL NOELIA</t>
-  </si>
-  <si>
-    <t>SÍNTESIS DE CIRCUITOS</t>
-  </si>
-  <si>
-    <t>LIC.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VILLA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CABERO </t>
-  </si>
-  <si>
-    <t>MARITZA</t>
-  </si>
-  <si>
-    <t>INVESTIGACIÓN OPERATIVA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YAÑIQUEZ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAGNE </t>
-  </si>
-  <si>
-    <t>CLAUDIA</t>
-  </si>
-  <si>
-    <t>PROGRAMACIÓN DE SISTEMAS I</t>
-  </si>
-  <si>
-    <t>12:00-13:30</t>
-  </si>
-  <si>
-    <t>MÉTODOS NUMÉRICOS</t>
-  </si>
-  <si>
-    <t>12:00-14:15</t>
-  </si>
-  <si>
     <t>ELECTRÓNICA ANALÓGICA II</t>
   </si>
   <si>
@@ -306,12 +309,12 @@
     <t>ELECTRONICA DIGITAL</t>
   </si>
   <si>
+    <t>10:00-12:45</t>
+  </si>
+  <si>
     <t>11:00-12:30</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>MAGUEÑO</t>
   </si>
   <si>
@@ -375,6 +378,9 @@
     <t>6TO.</t>
   </si>
   <si>
+    <t>9:15-12:45</t>
+  </si>
+  <si>
     <t>SANTOS</t>
   </si>
   <si>
@@ -576,10 +582,13 @@
     <t>SISTEMAS Y SERVICIOS DIGITALES</t>
   </si>
   <si>
-    <t>9:15-12:45</t>
-  </si>
-  <si>
-    <t>10:00-12:45</t>
+    <t>ING. DE SISTEMAS</t>
+  </si>
+  <si>
+    <t>ING. DE MECATRONICA</t>
+  </si>
+  <si>
+    <t>ING. DE SISTEMAS ELECTRONICOS</t>
   </si>
 </sst>
 </file>
@@ -589,7 +598,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -704,64 +713,64 @@
     </border>
   </borders>
   <cellStyleXfs count="11">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" applyFill="0" borderId="0" applyProtection="0" applyAlignment="0"/>
+    <xf numFmtId="43" applyNumberFormat="1" fontId="1" applyFont="0" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="2" applyFont="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" applyFont="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" applyFont="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" applyFont="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" applyFont="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" applyFont="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" applyFont="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" applyFont="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" applyFont="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" applyFill="0" borderId="0" xfId="0" applyProtection="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1"/>
+    <xf numFmtId="20" applyNumberFormat="1" fontId="4" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyBorder="1" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" applyFont="1" fillId="0" borderId="1" applyBorder="1" xfId="7" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" applyFont="1" fillId="3" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" applyFont="1" fillId="3" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" applyFont="1" fillId="0" borderId="1" applyBorder="1" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" applyFont="1" fillId="0" borderId="1" applyBorder="1" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" applyFont="1" fillId="3" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" applyFont="1" fillId="3" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" applyFont="1" fillId="0" borderId="1" applyBorder="1" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" applyFont="1" fillId="0" borderId="1" applyBorder="1" xfId="4" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" applyFont="1" fillId="3" applyFill="1" borderId="1" applyBorder="1" xfId="4" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" applyFont="1" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" applyFont="1" fillId="0" applyFill="1" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Millares 2 2" xfId="1"/>
@@ -1054,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G34" zoomScale="88" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="88" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,7 +1082,7 @@
     <col min="17" max="17" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" ht="39.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1129,7 +1138,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="2" ht="25.5">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1175,11 +1184,15 @@
       <c r="O2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="1"/>
+      <c r="P2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="3" ht="25.5">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1187,13 +1200,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F3" s="16">
         <v>579580</v>
@@ -1202,7 +1215,7 @@
         <v>22</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>24</v>
@@ -1214,36 +1227,40 @@
         <v>4</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="4" ht="25.5">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F4" s="16">
         <v>6106624</v>
@@ -1252,7 +1269,7 @@
         <v>22</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I4" s="8" t="s">
         <v>24</v>
@@ -1267,19 +1284,23 @@
         <v>28</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="5" ht="25.5">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1287,13 +1308,13 @@
         <v>18</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F5" s="16">
         <v>1707959</v>
@@ -1302,7 +1323,7 @@
         <v>22</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I5" s="8" t="s">
         <v>24</v>
@@ -1317,33 +1338,37 @@
         <v>26</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" ht="27" customHeight="1">
       <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F6" s="16">
         <v>2358779</v>
@@ -1352,7 +1377,7 @@
         <v>22</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="I6" s="8" t="s">
         <v>24</v>
@@ -1364,22 +1389,26 @@
         <v>3</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>28</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="7" ht="25.5">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1387,13 +1416,13 @@
         <v>18</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F7" s="15">
         <v>4288483</v>
@@ -1402,7 +1431,7 @@
         <v>22</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I7" s="10" t="s">
         <v>24</v>
@@ -1417,33 +1446,37 @@
         <v>28</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="R7" s="1"/>
     </row>
-    <row r="8" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="8" ht="25.5">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F8" s="16">
         <v>6157321</v>
@@ -1452,10 +1485,10 @@
         <v>22</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>25</v>
@@ -1467,33 +1500,37 @@
         <v>26</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>28</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="9" ht="25.5">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F9" s="16">
         <v>3660493</v>
@@ -1502,10 +1539,10 @@
         <v>22</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>25</v>
@@ -1514,22 +1551,26 @@
         <v>3</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="R9" s="1"/>
     </row>
-    <row r="10" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="10" ht="25.5">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1555,7 +1596,7 @@
         <v>75</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>25</v>
@@ -1564,26 +1605,26 @@
         <v>2</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="R10" s="1"/>
     </row>
-    <row r="11" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="11" ht="25.5">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1609,7 +1650,7 @@
         <v>80</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>25</v>
@@ -1621,24 +1662,28 @@
         <v>28</v>
       </c>
       <c r="M11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="N11" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="O11" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="R11" s="1"/>
     </row>
-    <row r="12" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" ht="25.5">
+      <c r="A12" s="0">
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>81</v>
@@ -1659,42 +1704,48 @@
         <v>84</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="0">
         <v>2</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="M12" t="s">
-        <v>49</v>
-      </c>
-      <c r="N12" t="s">
-        <v>36</v>
-      </c>
-      <c r="O12" t="s">
+      <c r="M12" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="N12" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="O12" s="0" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="P12" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q12" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" ht="25.5">
+      <c r="A13" s="0">
         <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F13" s="16">
         <v>4288483</v>
@@ -1706,12 +1757,12 @@
         <v>86</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="0">
         <v>6</v>
       </c>
       <c r="L13" s="17" t="s">
@@ -1721,27 +1772,33 @@
         <v>87</v>
       </c>
       <c r="N13" s="18" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="O13" s="17" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A14">
+        <v>88</v>
+      </c>
+      <c r="P13" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q13" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" ht="25.5">
+      <c r="A14" s="0">
         <v>13</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F14" s="16">
         <v>6157321</v>
@@ -1750,45 +1807,51 @@
         <v>22</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="0">
         <v>3</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L14" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="M14" t="s">
-        <v>37</v>
-      </c>
-      <c r="N14" t="s">
-        <v>34</v>
-      </c>
-      <c r="O14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="M14" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="N14" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="O14" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="P14" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q14" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" ht="25.5">
       <c r="A15" s="4">
         <v>14</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F15" s="16">
         <v>3382860</v>
@@ -1797,37 +1860,37 @@
         <v>22</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="0">
         <v>5</v>
       </c>
       <c r="L15" s="17" t="s">
         <v>28</v>
       </c>
       <c r="M15" s="18" t="s">
-        <v>186</v>
+        <v>96</v>
       </c>
       <c r="N15" s="18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O15" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="P15" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+      <c r="P15" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q15" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" ht="25.5">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -1835,13 +1898,13 @@
         <v>76</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F16" s="16">
         <v>4811736</v>
@@ -1850,31 +1913,37 @@
         <v>22</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K16">
+      <c r="K16" s="0">
         <v>3</v>
       </c>
       <c r="L16" s="18" t="s">
         <v>28</v>
       </c>
       <c r="M16" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="N16" t="s">
-        <v>96</v>
-      </c>
-      <c r="O16" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="N16" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="O16" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="P16" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q16" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" ht="25.5">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1882,13 +1951,13 @@
         <v>18</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>20</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F17" s="16">
         <v>2679320</v>
@@ -1897,45 +1966,51 @@
         <v>22</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="0">
         <v>5</v>
       </c>
       <c r="L17" s="18" t="s">
         <v>26</v>
       </c>
       <c r="M17" s="18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="N17" s="18" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="O17" s="18" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="P17" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q17" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" ht="38.25">
       <c r="A18" s="4">
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F18" s="16">
         <v>2227789</v>
@@ -1944,45 +2019,51 @@
         <v>22</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="0">
         <v>5</v>
       </c>
       <c r="L18" s="18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M18" s="18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N18" s="18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O18" s="18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="P18" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q18" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" ht="25.5">
       <c r="A19" s="4">
         <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F19" s="16">
         <v>3697276</v>
@@ -1991,31 +2072,37 @@
         <v>22</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="0">
         <v>4</v>
       </c>
       <c r="L19" s="18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M19" s="18" t="s">
         <v>29</v>
       </c>
       <c r="N19" s="18" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="O19" s="18" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="P19" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q19" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" ht="25.5">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2023,46 +2110,52 @@
         <v>18</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G20" s="12" t="s">
         <v>22</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="0">
         <v>4</v>
       </c>
       <c r="L20" s="18" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="M20" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="N20" t="s">
-        <v>96</v>
-      </c>
-      <c r="O20" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="N20" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="O20" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="P20" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q20" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" ht="25.5">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2070,13 +2163,13 @@
         <v>18</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F21" s="16">
         <v>4793659</v>
@@ -2085,31 +2178,37 @@
         <v>22</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K21">
+      <c r="K21" s="0">
         <v>4</v>
       </c>
       <c r="L21" s="18" t="s">
         <v>28</v>
       </c>
       <c r="M21" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="N21" t="s">
-        <v>96</v>
-      </c>
-      <c r="O21" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="N21" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="O21" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="P21" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q21" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" ht="25.5">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2117,13 +2216,13 @@
         <v>18</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>20</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F22" s="16">
         <v>2679320</v>
@@ -2132,31 +2231,37 @@
         <v>22</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K22">
+      <c r="K22" s="0">
         <v>4</v>
       </c>
       <c r="L22" s="18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M22" s="18" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N22" s="17" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="O22" s="18" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="P22" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q22" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" ht="25.5">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2164,13 +2269,13 @@
         <v>18</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F23" s="16">
         <v>2288375</v>
@@ -2179,45 +2284,51 @@
         <v>22</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K23">
+      <c r="K23" s="0">
         <v>5</v>
       </c>
       <c r="L23" s="18" t="s">
         <v>26</v>
       </c>
       <c r="M23" s="18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N23" s="18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="O23" s="18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="P23" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q23" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" ht="25.5">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F24" s="16">
         <v>3697276</v>
@@ -2226,15 +2337,15 @@
         <v>22</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K24">
+      <c r="K24" s="0">
         <v>4</v>
       </c>
       <c r="L24" s="18" t="s">
@@ -2247,24 +2358,30 @@
         <v>28</v>
       </c>
       <c r="O24" s="18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A25">
+        <v>57</v>
+      </c>
+      <c r="P24" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q24" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" ht="25.5">
+      <c r="A25" s="0">
         <v>24</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="F25" s="16">
         <v>3330918</v>
@@ -2273,92 +2390,104 @@
         <v>22</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K25">
+      <c r="K25" s="0">
         <v>4</v>
       </c>
       <c r="L25" s="17" t="s">
         <v>26</v>
       </c>
       <c r="M25" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="N25" s="18" t="s">
         <v>35</v>
-      </c>
-      <c r="N25" s="18" t="s">
-        <v>34</v>
       </c>
       <c r="O25" s="18" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="P25" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q25" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" ht="25.5">
+      <c r="A26" s="0">
         <v>25</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G26" s="12" t="s">
         <v>22</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K26">
+      <c r="K26" s="0">
         <v>4</v>
       </c>
       <c r="L26" s="17" t="s">
         <v>26</v>
       </c>
       <c r="M26" s="18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="N26" s="18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="O26" s="18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A27">
+        <v>45</v>
+      </c>
+      <c r="P26" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q26" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" ht="25.5">
+      <c r="A27" s="0">
         <v>26</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F27" s="16">
         <v>2288375</v>
@@ -2367,31 +2496,37 @@
         <v>22</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K27">
+      <c r="K27" s="0">
         <v>5</v>
       </c>
       <c r="L27" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M27" s="18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="N27" s="18" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="O27" s="18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="P27" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q27" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" ht="25.5">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -2399,60 +2534,66 @@
         <v>76</v>
       </c>
       <c r="C28" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="I28" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="D28" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="F28" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="H28" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="I28" s="8" t="s">
-        <v>138</v>
-      </c>
       <c r="J28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K28">
+      <c r="K28" s="0">
         <v>3</v>
       </c>
       <c r="L28" s="17" t="s">
         <v>28</v>
       </c>
       <c r="M28" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="N28" t="s">
-        <v>96</v>
-      </c>
-      <c r="O28" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="N28" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="O28" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="P28" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q28" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" ht="25.5">
       <c r="A29" s="4">
         <v>28</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F29" s="16">
         <v>3697276</v>
@@ -2461,45 +2602,51 @@
         <v>22</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K29">
+      <c r="K29" s="0">
         <v>5</v>
       </c>
       <c r="L29" s="17" t="s">
         <v>26</v>
       </c>
       <c r="M29" s="18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N29" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="O29" s="18" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="P29" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q29" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" ht="38.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F30" s="16">
         <v>2227789</v>
@@ -2508,45 +2655,51 @@
         <v>22</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K30">
+      <c r="K30" s="0">
         <v>5</v>
       </c>
       <c r="L30" s="17" t="s">
         <v>28</v>
       </c>
       <c r="M30" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="N30" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="N30" s="17" t="s">
-        <v>36</v>
-      </c>
       <c r="O30" s="18" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="P30" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q30" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" ht="25.5">
       <c r="A31" s="4">
         <v>30</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F31" s="16">
         <v>2319203</v>
@@ -2555,15 +2708,15 @@
         <v>22</v>
       </c>
       <c r="H31" s="13" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K31">
+      <c r="K31" s="0">
         <v>4</v>
       </c>
       <c r="L31" s="17" t="s">
@@ -2573,48 +2726,54 @@
         <v>29</v>
       </c>
       <c r="N31" s="17" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="O31" s="18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="P31" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q31" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" ht="25.5">
       <c r="A32" s="4">
         <v>31</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G32" s="12" t="s">
         <v>22</v>
       </c>
       <c r="H32" s="14" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="I32" s="10" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K32">
+      <c r="K32" s="0">
         <v>6</v>
       </c>
       <c r="L32" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M32" s="18" t="s">
         <v>85</v>
@@ -2623,10 +2782,16 @@
         <v>28</v>
       </c>
       <c r="O32" s="18" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+      <c r="P32" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q32" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" ht="25.5">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2634,30 +2799,30 @@
         <v>18</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F33" s="16" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G33" s="12" t="s">
         <v>22</v>
       </c>
       <c r="H33" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="I33" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="I33" s="8" t="s">
-        <v>156</v>
-      </c>
       <c r="J33" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K33">
+      <c r="K33" s="0">
         <v>5</v>
       </c>
       <c r="L33" s="17" t="s">
@@ -2667,13 +2832,19 @@
         <v>85</v>
       </c>
       <c r="N33" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="O33" s="18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="P33" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q33" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" ht="25.5">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2681,13 +2852,13 @@
         <v>18</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="F34" s="16">
         <v>3497104</v>
@@ -2696,45 +2867,51 @@
         <v>22</v>
       </c>
       <c r="H34" s="13" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K34">
+      <c r="K34" s="0">
         <v>5</v>
       </c>
       <c r="L34" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M34" s="18" t="s">
         <v>85</v>
       </c>
       <c r="N34" s="17" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="O34" s="18" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="P34" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q34" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" ht="25.5">
       <c r="A35" s="1">
         <v>34</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F35" s="16">
         <v>6157321</v>
@@ -2743,31 +2920,37 @@
         <v>22</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K35">
+      <c r="K35" s="0">
         <v>4</v>
       </c>
       <c r="L35" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M35" s="18" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N35" s="17" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="O35" s="18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="P35" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q35" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" ht="25.5">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2775,13 +2958,13 @@
         <v>18</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="F36" s="16">
         <v>1845009</v>
@@ -2790,31 +2973,37 @@
         <v>22</v>
       </c>
       <c r="H36" s="13" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K36">
+      <c r="K36" s="0">
         <v>5</v>
       </c>
       <c r="L36" s="17" t="s">
         <v>26</v>
       </c>
       <c r="M36" s="18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N36" s="17" t="s">
         <v>28</v>
       </c>
       <c r="O36" s="18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="P36" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q36" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" ht="25.5">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2822,13 +3011,13 @@
         <v>18</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="F37" s="16">
         <v>4284954</v>
@@ -2837,45 +3026,51 @@
         <v>22</v>
       </c>
       <c r="H37" s="13" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K37">
+      <c r="K37" s="0">
         <v>5</v>
       </c>
       <c r="L37" s="17" t="s">
         <v>26</v>
       </c>
       <c r="M37" s="18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="N37" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O37" s="18" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="P37" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q37" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" ht="25.5">
+      <c r="A38" s="0">
         <v>37</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="F38" s="16">
         <v>2364316</v>
@@ -2884,15 +3079,15 @@
         <v>22</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K38">
+      <c r="K38" s="0">
         <v>7</v>
       </c>
       <c r="L38" s="17" t="s">
@@ -2905,24 +3100,30 @@
         <v>28</v>
       </c>
       <c r="O38" s="18" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A39">
+        <v>178</v>
+      </c>
+      <c r="P38" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q38" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" ht="25.5">
+      <c r="A39" s="0">
         <v>38</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F39" s="16">
         <v>4992347</v>
@@ -2931,15 +3132,15 @@
         <v>22</v>
       </c>
       <c r="H39" s="13" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K39">
+      <c r="K39" s="0">
         <v>5</v>
       </c>
       <c r="L39" s="17" t="s">
@@ -2949,27 +3150,33 @@
         <v>85</v>
       </c>
       <c r="N39" s="17" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="O39" s="18" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="P39" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q39" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" ht="25.5">
+      <c r="A40" s="0">
         <v>39</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="F40" s="16">
         <v>3497104</v>
@@ -2978,45 +3185,51 @@
         <v>22</v>
       </c>
       <c r="H40" s="13" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K40">
+      <c r="K40" s="0">
         <v>5</v>
       </c>
       <c r="L40" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M40" s="18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N40" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O40" s="18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="P40" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q40" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" ht="25.5">
       <c r="A41" s="4">
         <v>40</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F41" s="16">
         <v>3660493</v>
@@ -3025,45 +3238,51 @@
         <v>22</v>
       </c>
       <c r="H41" s="13" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K41">
+      <c r="K41" s="0">
         <v>6</v>
       </c>
       <c r="L41" s="17" t="s">
         <v>26</v>
       </c>
       <c r="M41" s="18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N41" s="17" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="O41" s="18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="P41" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q41" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" ht="38.25">
       <c r="A42" s="4">
         <v>41</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F42" s="16">
         <v>2227789</v>
@@ -3072,85 +3291,411 @@
         <v>22</v>
       </c>
       <c r="H42" s="13" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="J42" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K42">
+      <c r="K42" s="0">
         <v>4</v>
       </c>
       <c r="L42" s="17" t="s">
         <v>26</v>
       </c>
       <c r="M42" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="N42" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="O42" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="P42" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q42" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0">
+        <v>42</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F43" s="15">
+        <v>4288483</v>
+      </c>
+      <c r="G43" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="H43" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="I43" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K43" s="1">
+        <v>2</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N43" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="O43" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P43" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q43" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="R43" s="1"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="4">
+        <v>43</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F44" s="16">
+        <v>6157321</v>
+      </c>
+      <c r="G44" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="H44" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="I44" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K44" s="1">
+        <v>4</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O44" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P44" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q44" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="R44" s="1"/>
+    </row>
+    <row r="45" ht="38.25">
+      <c r="A45" s="4">
         <v>44</v>
       </c>
-      <c r="N42" s="17" t="s">
+      <c r="B45" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F45" s="16">
+        <v>2227789</v>
+      </c>
+      <c r="G45" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="H45" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="I45" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K45" s="0">
+        <v>5</v>
+      </c>
+      <c r="L45" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="M45" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="O42" s="18" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="9"/>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="9"/>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="9"/>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="9"/>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B47" s="8"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="9"/>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="9"/>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="N45" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="O45" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="P45" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q45" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0">
+        <v>45</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="F46" s="16">
+        <v>3697276</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="H46" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="I46" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K46" s="0">
+        <v>4</v>
+      </c>
+      <c r="L46" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="M46" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="N46" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="O46" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="P46" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q46" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" ht="38.25">
+      <c r="A47" s="4">
+        <v>44</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F47" s="16">
+        <v>2227789</v>
+      </c>
+      <c r="G47" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="H47" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="I47" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K47" s="0">
+        <v>5</v>
+      </c>
+      <c r="L47" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="M47" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="N47" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="O47" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48" ht="25.5">
+      <c r="A48" s="0">
+        <v>45</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="F48" s="16">
+        <v>3697276</v>
+      </c>
+      <c r="G48" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="H48" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="I48" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K48" s="0">
+        <v>4</v>
+      </c>
+      <c r="L48" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="M48" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="N48" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="O48" s="18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0">
+        <v>48</v>
+      </c>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
       <c r="E49" s="9"/>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="K49" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="L49" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="M49" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="N49" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="O49" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="P49" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q49" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="4">
+        <v>49</v>
+      </c>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
       <c r="E50" s="9"/>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="K50" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="L50" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="M50" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="N50" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="O50" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="P50" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q50" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="51">
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
       <c r="D51" s="8"/>
       <c r="E51" s="9"/>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="52">
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
@@ -3158,5 +3703,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>